<commit_message>
Rename arguments of measure add_temperature_setpoints to conform to OS style and to improve clarity.
</commit_message>
<xml_diff>
--- a/docs/Measure_Arguments.xlsx
+++ b/docs/Measure_Arguments.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="120">
   <si>
     <t>Measure</t>
   </si>
@@ -348,6 +348,45 @@
   </si>
   <si>
     <t>The type of ventilation system. One of: 1, 2</t>
+  </si>
+  <si>
+    <t>add_temperature_setpoints</t>
+  </si>
+  <si>
+    <t>heating_temp_selection</t>
+  </si>
+  <si>
+    <t>Selection of heating temperature</t>
+  </si>
+  <si>
+    <t>(Export only) Selection of heating temperature</t>
+  </si>
+  <si>
+    <t>cooling_temp_selection</t>
+  </si>
+  <si>
+    <t>Selection of cooling temperature</t>
+  </si>
+  <si>
+    <t>(Export only) Selection of cooling temperature</t>
+  </si>
+  <si>
+    <t>is_custom_heating</t>
+  </si>
+  <si>
+    <t>Is custom heating temperature</t>
+  </si>
+  <si>
+    <t>(Export only) Flag whether the selected heating temperature is a custom schedule</t>
+  </si>
+  <si>
+    <t>is_custom_cooling</t>
+  </si>
+  <si>
+    <t>Is custom cooling temperature</t>
+  </si>
+  <si>
+    <t>(Export only) Flag whether the selectedcooling temperature is a custom schedule</t>
   </si>
 </sst>
 </file>
@@ -666,19 +705,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="94.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1145,7 +1186,7 @@
         <v>80</v>
       </c>
       <c r="G22" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1325,6 +1366,266 @@
       </c>
       <c r="H29">
         <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" t="s">
+        <v>110</v>
+      </c>
+      <c r="G39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s">
+        <v>113</v>
+      </c>
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" t="s">
+        <v>116</v>
+      </c>
+      <c r="G41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename arguments of measure add_internal_loads to conform to OS style and to improve clarity.
</commit_message>
<xml_diff>
--- a/docs/Measure_Arguments.xlsx
+++ b/docs/Measure_Arguments.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="215">
   <si>
     <t>Measure</t>
   </si>
@@ -387,6 +387,291 @@
   </si>
   <si>
     <t>(Export only) Flag whether the selectedcooling temperature is a custom schedule</t>
+  </si>
+  <si>
+    <t>add_internal_loads</t>
+  </si>
+  <si>
+    <t>electric_equipment_sched_weekday</t>
+  </si>
+  <si>
+    <t>Electric equipment schedule for weekdays</t>
+  </si>
+  <si>
+    <t>Schedule for the internal load of electric equipment for weekdays.</t>
+  </si>
+  <si>
+    <t>electric_equipment_sched_saturday</t>
+  </si>
+  <si>
+    <t>Electric equipment schedule for saturday</t>
+  </si>
+  <si>
+    <t>Schedule for the internal load of electric equipment for holidays.</t>
+  </si>
+  <si>
+    <t>electric_equipment_sched_sunday</t>
+  </si>
+  <si>
+    <t>Electric equipment schedule for sunday</t>
+  </si>
+  <si>
+    <t>Schedule for the internal load of electric equipment for sunday.</t>
+  </si>
+  <si>
+    <t>electric_equipment_sched_holiday</t>
+  </si>
+  <si>
+    <t>Electric equipment schedule for holidays</t>
+  </si>
+  <si>
+    <t>Lighting schedule for weekdays</t>
+  </si>
+  <si>
+    <t>Schedule for the internal load of lighting for weekdays.</t>
+  </si>
+  <si>
+    <t>Lighting schedule for saturday</t>
+  </si>
+  <si>
+    <t>Schedule for the internal load of lighting for saturday.</t>
+  </si>
+  <si>
+    <t>Lighting schedule for sunday</t>
+  </si>
+  <si>
+    <t>Schedule for the internal load of lighting for sunday.</t>
+  </si>
+  <si>
+    <t>Lighting schedule for holiday</t>
+  </si>
+  <si>
+    <t>Schedule for the internal load of lighting for holiday.</t>
+  </si>
+  <si>
+    <t>people_sched_weekday</t>
+  </si>
+  <si>
+    <t>People schedule for weekdays</t>
+  </si>
+  <si>
+    <t>Schedule for the presence of people for weekdays.</t>
+  </si>
+  <si>
+    <t>Schedule for the presence of people for saturday.</t>
+  </si>
+  <si>
+    <t>Schedule for the presence of people for sunday.</t>
+  </si>
+  <si>
+    <t>Schedule for the presence of people for holidays.</t>
+  </si>
+  <si>
+    <t>People schedule for holiday</t>
+  </si>
+  <si>
+    <t>People schedule for saturday</t>
+  </si>
+  <si>
+    <t>People schedule for sunday</t>
+  </si>
+  <si>
+    <t>people_sched_saturday</t>
+  </si>
+  <si>
+    <t>people_sched_sunday</t>
+  </si>
+  <si>
+    <t>people_sched_holiday</t>
+  </si>
+  <si>
+    <t>people_activity_sched_weekday</t>
+  </si>
+  <si>
+    <t>People activity schedule for weekdays</t>
+  </si>
+  <si>
+    <t>Schedule for the activity of people for weekdays.</t>
+  </si>
+  <si>
+    <t>people_activity_sched_satuday</t>
+  </si>
+  <si>
+    <t>People activity schedule for saturday</t>
+  </si>
+  <si>
+    <t>Schedule for the activity of people for saturday.</t>
+  </si>
+  <si>
+    <t>people_activity_sched_sunday</t>
+  </si>
+  <si>
+    <t>People activity schedule for sunday</t>
+  </si>
+  <si>
+    <t>Schedule for the activity of people for sunday.</t>
+  </si>
+  <si>
+    <t>people_activity_sched_holiday</t>
+  </si>
+  <si>
+    <t>People activity schedule for holiday</t>
+  </si>
+  <si>
+    <t>Schedule for the activity of people for holidays.</t>
+  </si>
+  <si>
+    <t>electric_equipment_power_per_floor_area</t>
+  </si>
+  <si>
+    <t>Area-specific electric equipment power</t>
+  </si>
+  <si>
+    <t>kWh/m^-2</t>
+  </si>
+  <si>
+    <t>Power of electric equipment relative to the GFA.</t>
+  </si>
+  <si>
+    <t>lighting_power_per_floor_area</t>
+  </si>
+  <si>
+    <t>Power of artificial lighting relative to the GFA.</t>
+  </si>
+  <si>
+    <t>floor_area_per_person</t>
+  </si>
+  <si>
+    <t>GFA per person</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>Area-specific artificial lighting power</t>
+  </si>
+  <si>
+    <t>area_gfa_import</t>
+  </si>
+  <si>
+    <t>GFA of imported model</t>
+  </si>
+  <si>
+    <t>Selection of standard ratio of NFA over GFA</t>
+  </si>
+  <si>
+    <t>nfa_gfa_ratio_selection</t>
+  </si>
+  <si>
+    <t>electric_equipment_sched_selection</t>
+  </si>
+  <si>
+    <t>Selection of the electrip equipment schedule</t>
+  </si>
+  <si>
+    <t>lighting_sched_selection</t>
+  </si>
+  <si>
+    <t>Selection of the artificial lighting schedule</t>
+  </si>
+  <si>
+    <t>people_sched_selection</t>
+  </si>
+  <si>
+    <t>Selection of the people schedule</t>
+  </si>
+  <si>
+    <t>people_activity_sched_selection</t>
+  </si>
+  <si>
+    <t>Selection of the people activity schedule</t>
+  </si>
+  <si>
+    <t>(Export only) Selection of the people activity schedule.</t>
+  </si>
+  <si>
+    <t>(Export only) Selection of the people presence schedule.</t>
+  </si>
+  <si>
+    <t>(Export only) Selection of the artificial lighting schedule.</t>
+  </si>
+  <si>
+    <t>(Export only) Selection of the electric equipment schedule.</t>
+  </si>
+  <si>
+    <t>(Export only) Selection of standard ratio of NFA over GFA.</t>
+  </si>
+  <si>
+    <t>(Export only) GFA of the imported model, if any.</t>
+  </si>
+  <si>
+    <t>GFA per person.</t>
+  </si>
+  <si>
+    <t>is_custom_ratio</t>
+  </si>
+  <si>
+    <t>Is custom NFA over GFA ratio</t>
+  </si>
+  <si>
+    <t>(Export only) Flag whether the ratio of NFA over GFA is custom.</t>
+  </si>
+  <si>
+    <t>is_imported_model</t>
+  </si>
+  <si>
+    <t>Is imported model</t>
+  </si>
+  <si>
+    <t>(Export only) Flag whether the geometric model is imported.</t>
+  </si>
+  <si>
+    <t>is_custom_electric equipment</t>
+  </si>
+  <si>
+    <t>Is custom electric equipment schedule</t>
+  </si>
+  <si>
+    <t>(Export only) Flag whether the electric equipment schedule is custom.</t>
+  </si>
+  <si>
+    <t>is_custom_lighting</t>
+  </si>
+  <si>
+    <t>Is custom lighting schedule</t>
+  </si>
+  <si>
+    <t>(Export only) Flag whether the artificial lighting schedule is custom.</t>
+  </si>
+  <si>
+    <t>is_custom_people</t>
+  </si>
+  <si>
+    <t>Is custom people schedule</t>
+  </si>
+  <si>
+    <t>(Export only) Flag whether the people schedule is custom.</t>
+  </si>
+  <si>
+    <t>is_custom_people_activity</t>
+  </si>
+  <si>
+    <t>Is custom people activity</t>
+  </si>
+  <si>
+    <t>(Export only) Flag whether the people activity schedule is custom.</t>
+  </si>
+  <si>
+    <t>lighting_sched_weekday</t>
+  </si>
+  <si>
+    <t>lighting_sched_saturday</t>
+  </si>
+  <si>
+    <t>lighting_sched_sunday</t>
+  </si>
+  <si>
+    <t>lighting_sched_holiday</t>
   </si>
 </sst>
 </file>
@@ -705,10 +990,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,6 +1913,661 @@
         <v>37</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" t="s">
+        <v>123</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" t="s">
+        <v>126</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s">
+        <v>126</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
+        <v>133</v>
+      </c>
+      <c r="G47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" t="s">
+        <v>135</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" t="s">
+        <v>213</v>
+      </c>
+      <c r="C49" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
+        <v>137</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" t="s">
+        <v>214</v>
+      </c>
+      <c r="C50" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
+        <v>139</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
+        <v>142</v>
+      </c>
+      <c r="G51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" t="s">
+        <v>149</v>
+      </c>
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
+        <v>143</v>
+      </c>
+      <c r="G52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
+        <v>144</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" t="s">
+        <v>151</v>
+      </c>
+      <c r="C54" t="s">
+        <v>146</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>145</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" t="s">
+        <v>153</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" t="s">
+        <v>154</v>
+      </c>
+      <c r="G55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
+        <v>155</v>
+      </c>
+      <c r="C56" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" t="s">
+        <v>157</v>
+      </c>
+      <c r="G56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>160</v>
+      </c>
+      <c r="G57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" t="s">
+        <v>161</v>
+      </c>
+      <c r="C58" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" t="s">
+        <v>163</v>
+      </c>
+      <c r="G58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" t="s">
+        <v>166</v>
+      </c>
+      <c r="F60" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s">
+        <v>166</v>
+      </c>
+      <c r="F61" t="s">
+        <v>169</v>
+      </c>
+      <c r="G61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" t="s">
+        <v>171</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" t="s">
+        <v>172</v>
+      </c>
+      <c r="F62" t="s">
+        <v>192</v>
+      </c>
+      <c r="G62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" t="s">
+        <v>174</v>
+      </c>
+      <c r="C63" t="s">
+        <v>175</v>
+      </c>
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" t="s">
+        <v>172</v>
+      </c>
+      <c r="F63" t="s">
+        <v>191</v>
+      </c>
+      <c r="G63" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" t="s">
+        <v>176</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>190</v>
+      </c>
+      <c r="G64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" t="s">
+        <v>178</v>
+      </c>
+      <c r="C65" t="s">
+        <v>179</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
+        <v>189</v>
+      </c>
+      <c r="G65" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" t="s">
+        <v>181</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" t="s">
+        <v>188</v>
+      </c>
+      <c r="G66" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" t="s">
+        <v>182</v>
+      </c>
+      <c r="C67" t="s">
+        <v>183</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" t="s">
+        <v>187</v>
+      </c>
+      <c r="G67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" t="s">
+        <v>184</v>
+      </c>
+      <c r="C68" t="s">
+        <v>185</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" t="s">
+        <v>186</v>
+      </c>
+      <c r="G68" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" t="s">
+        <v>193</v>
+      </c>
+      <c r="C69" t="s">
+        <v>194</v>
+      </c>
+      <c r="D69" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" t="s">
+        <v>195</v>
+      </c>
+      <c r="G69" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" t="s">
+        <v>197</v>
+      </c>
+      <c r="D70" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" t="s">
+        <v>198</v>
+      </c>
+      <c r="G70" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" t="s">
+        <v>199</v>
+      </c>
+      <c r="C71" t="s">
+        <v>200</v>
+      </c>
+      <c r="D71" t="s">
+        <v>40</v>
+      </c>
+      <c r="F71" t="s">
+        <v>201</v>
+      </c>
+      <c r="G71" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" t="s">
+        <v>202</v>
+      </c>
+      <c r="C72" t="s">
+        <v>203</v>
+      </c>
+      <c r="D72" t="s">
+        <v>40</v>
+      </c>
+      <c r="F72" t="s">
+        <v>204</v>
+      </c>
+      <c r="G72" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>120</v>
+      </c>
+      <c r="B73" t="s">
+        <v>205</v>
+      </c>
+      <c r="C73" t="s">
+        <v>206</v>
+      </c>
+      <c r="D73" t="s">
+        <v>40</v>
+      </c>
+      <c r="F73" t="s">
+        <v>207</v>
+      </c>
+      <c r="G73" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>120</v>
+      </c>
+      <c r="B74" t="s">
+        <v>208</v>
+      </c>
+      <c r="C74" t="s">
+        <v>209</v>
+      </c>
+      <c r="D74" t="s">
+        <v>40</v>
+      </c>
+      <c r="F74" t="s">
+        <v>210</v>
+      </c>
+      <c r="G74" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H9"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rename arguments of measure add_materials_and_construction to comply with OS style and to improve clarity.
</commit_message>
<xml_diff>
--- a/docs/Measure_Arguments.xlsx
+++ b/docs/Measure_Arguments.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="340">
   <si>
     <t>Measure</t>
   </si>
@@ -527,9 +527,6 @@
     <t>Area-specific electric equipment power</t>
   </si>
   <si>
-    <t>kWh/m^-2</t>
-  </si>
-  <si>
     <t>Power of electric equipment relative to the GFA.</t>
   </si>
   <si>
@@ -672,6 +669,384 @@
   </si>
   <si>
     <t>lighting_sched_holiday</t>
+  </si>
+  <si>
+    <t>add_materials_and_construction</t>
+  </si>
+  <si>
+    <t>external_wall_$i_name</t>
+  </si>
+  <si>
+    <t>Name of layer $i of external walls</t>
+  </si>
+  <si>
+    <t>Name of layer $i for the external wall construction</t>
+  </si>
+  <si>
+    <t>external_wall_$i_thickness</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i of external walls</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i for the external wall construction</t>
+  </si>
+  <si>
+    <t>external_wall_$i_conductivity</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i of external walls</t>
+  </si>
+  <si>
+    <t>W/m*K</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i for the external wall construction</t>
+  </si>
+  <si>
+    <t>external_wall_$i_density</t>
+  </si>
+  <si>
+    <t>Density of layer $i of external walls</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>Density of layer $i for the external wall construction</t>
+  </si>
+  <si>
+    <t>Heat capacity of layer $i of external walls</t>
+  </si>
+  <si>
+    <t>external_wall_$i_heat_capacity</t>
+  </si>
+  <si>
+    <t>kW*h/m^-2</t>
+  </si>
+  <si>
+    <t>Mass-specific heat capacity of layer $i for the external wall construction</t>
+  </si>
+  <si>
+    <t>J/kg*K</t>
+  </si>
+  <si>
+    <t>roof_$i_name</t>
+  </si>
+  <si>
+    <t>roof_$i_thickness</t>
+  </si>
+  <si>
+    <t>roof_$i_conductivity</t>
+  </si>
+  <si>
+    <t>roof_$i_density</t>
+  </si>
+  <si>
+    <t>roof_$i_heat_capacity</t>
+  </si>
+  <si>
+    <t>Name of layer $i of roof</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i of roof</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i of roof</t>
+  </si>
+  <si>
+    <t>Density of layer $i of roof</t>
+  </si>
+  <si>
+    <t>Heat capacity of layer $i of roof</t>
+  </si>
+  <si>
+    <t>Mass-specific heat capacity of layer $i for the roof construction</t>
+  </si>
+  <si>
+    <t>Name of layer $i for the roof construction</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i for the roof construction</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i for the roof construction</t>
+  </si>
+  <si>
+    <t>Density of layer $i for the roof construction</t>
+  </si>
+  <si>
+    <t>base_plate_$i_name</t>
+  </si>
+  <si>
+    <t>base_plate_$i_thickness</t>
+  </si>
+  <si>
+    <t>base_plate_$i_conductivity</t>
+  </si>
+  <si>
+    <t>base_plate_$i_density</t>
+  </si>
+  <si>
+    <t>base_plate_$i_heat_capacity</t>
+  </si>
+  <si>
+    <t>Name of layer $i of base plate</t>
+  </si>
+  <si>
+    <t>Name of layer $i for the base plate construction</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i of base plate</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i for the base plate construction</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i of base plate</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i for the base plate construction</t>
+  </si>
+  <si>
+    <t>Density of layer $i of base plate</t>
+  </si>
+  <si>
+    <t>Density of layer $i for the base plate construction</t>
+  </si>
+  <si>
+    <t>Heat capacity of layer $i of base plate</t>
+  </si>
+  <si>
+    <t>Mass-specific heat capacity of layer $i for the base plate construction</t>
+  </si>
+  <si>
+    <t>interior_slab_$i_name</t>
+  </si>
+  <si>
+    <t>interior_slab_$i_thickness</t>
+  </si>
+  <si>
+    <t>interior_slab_$i_conductivity</t>
+  </si>
+  <si>
+    <t>interior_slab_$i_density</t>
+  </si>
+  <si>
+    <t>interior_slab_$i_heat_capacity</t>
+  </si>
+  <si>
+    <t>Name of layer $i of interior slabs</t>
+  </si>
+  <si>
+    <t>Name of layer $i for the interior slabs construction</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i of interior slabs</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i for the interior slabs construction</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i of interior slabs</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i for the interior slabs construction</t>
+  </si>
+  <si>
+    <t>Density of layer $i of interior slabs</t>
+  </si>
+  <si>
+    <t>Density of layer $i for the interior slabs construction</t>
+  </si>
+  <si>
+    <t>Heat capacity of layer $i of interior slabs</t>
+  </si>
+  <si>
+    <t>Mass-specific heat capacity of layer $i for the interior slabs construction</t>
+  </si>
+  <si>
+    <t>inner_masses_$i_name</t>
+  </si>
+  <si>
+    <t>inner_masses_$i_thickness</t>
+  </si>
+  <si>
+    <t>inner_masses_$i_conductivity</t>
+  </si>
+  <si>
+    <t>inner_masses_$i_density</t>
+  </si>
+  <si>
+    <t>inner_masses_$i_heat_capacity</t>
+  </si>
+  <si>
+    <t>Name of layer $i of inner masses</t>
+  </si>
+  <si>
+    <t>Name of layer $i for the inner masses construction</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i of inner masses</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i for the inner masses construction</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i of inner masses</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i for the inner masses construction</t>
+  </si>
+  <si>
+    <t>Density of layer $i of inner masses</t>
+  </si>
+  <si>
+    <t>Density of layer $i for the inner masses construction</t>
+  </si>
+  <si>
+    <t>Heat capacity of layer $i of inner masses</t>
+  </si>
+  <si>
+    <t>Mass-specific heat capacity of layer $i for the inner masses construction</t>
+  </si>
+  <si>
+    <t>chilled_ceiling_$i_name</t>
+  </si>
+  <si>
+    <t>chilled_ceiling_$i_thickness</t>
+  </si>
+  <si>
+    <t>chilled_ceiling_$i_conductivity</t>
+  </si>
+  <si>
+    <t>chilled_ceiling_$i_density</t>
+  </si>
+  <si>
+    <t>chilled_ceiling_$i_heat_capacity</t>
+  </si>
+  <si>
+    <t>Name of layer $i of chilled ceiling</t>
+  </si>
+  <si>
+    <t>Name of layer $i for the chilled ceiling construction</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i of chilled ceiling</t>
+  </si>
+  <si>
+    <t>Thickness of layer $i for the chilled ceiling construction</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i of chilled ceiling</t>
+  </si>
+  <si>
+    <t>Heat conductivity of layer $i for the chilled ceiling construction</t>
+  </si>
+  <si>
+    <t>Density of layer $i of chilled ceiling</t>
+  </si>
+  <si>
+    <t>Density of layer $i for the chilled ceiling construction</t>
+  </si>
+  <si>
+    <t>Heat capacity of layer $i of chilled ceiling</t>
+  </si>
+  <si>
+    <t>Mass-specific heat capacity of layer $i for the chilled ceiling construction</t>
+  </si>
+  <si>
+    <t>chilled_ceiling_source_layer</t>
+  </si>
+  <si>
+    <t>Source layer of the chilled ceiling</t>
+  </si>
+  <si>
+    <t>The number of the layer of the chilled ceiling construction which performs the heat transfer.</t>
+  </si>
+  <si>
+    <t>chilled_ceiling_temp_calc_layer</t>
+  </si>
+  <si>
+    <t>Chilled ceiling temp calc layer</t>
+  </si>
+  <si>
+    <t>chilled_ceiling_dim_ctf</t>
+  </si>
+  <si>
+    <t>Chilled ceiling dim CTF</t>
+  </si>
+  <si>
+    <t>chilled_ceiling_tube_spacing</t>
+  </si>
+  <si>
+    <t>Spacing of tubes of the chilled ceiling</t>
+  </si>
+  <si>
+    <t>The spacing between tubes for the construction of chilled ceilings.</t>
+  </si>
+  <si>
+    <t>windows_name</t>
+  </si>
+  <si>
+    <t>Name of the windows construction</t>
+  </si>
+  <si>
+    <t>windows_u_value</t>
+  </si>
+  <si>
+    <t>U-value of the windows construction</t>
+  </si>
+  <si>
+    <t>windows_shgc</t>
+  </si>
+  <si>
+    <t>SHGC of the windows construction</t>
+  </si>
+  <si>
+    <t>Name of the windows construction.</t>
+  </si>
+  <si>
+    <t>U-value of the windows construction.</t>
+  </si>
+  <si>
+    <t>Chilled ceiling dim CTF.</t>
+  </si>
+  <si>
+    <t>Chilled ceiling temp calc layer.</t>
+  </si>
+  <si>
+    <t>construction_standard_selection</t>
+  </si>
+  <si>
+    <t>Selection value of the construction standard</t>
+  </si>
+  <si>
+    <t>(Export only) Selection value of the construction standard</t>
+  </si>
+  <si>
+    <t>is_custom_standard</t>
+  </si>
+  <si>
+    <t>Is custom standard</t>
+  </si>
+  <si>
+    <t>(Export only) Flag wheter the construction standard is custom</t>
+  </si>
+  <si>
+    <t>inner_masses_selection</t>
+  </si>
+  <si>
+    <t>Selection value of the inner masses</t>
+  </si>
+  <si>
+    <t>(Export only) Selection value of the inner masses construction.</t>
+  </si>
+  <si>
+    <t>Solar heat gain coefficient of the windows constructions.</t>
   </si>
 </sst>
 </file>
@@ -990,10 +1365,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,7 +2373,7 @@
         <v>120</v>
       </c>
       <c r="B47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C47" t="s">
         <v>132</v>
@@ -2018,7 +2393,7 @@
         <v>120</v>
       </c>
       <c r="B48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C48" t="s">
         <v>134</v>
@@ -2038,7 +2413,7 @@
         <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C49" t="s">
         <v>136</v>
@@ -2058,7 +2433,7 @@
         <v>120</v>
       </c>
       <c r="B50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C50" t="s">
         <v>138</v>
@@ -2270,10 +2645,10 @@
         <v>15</v>
       </c>
       <c r="E60" t="s">
+        <v>232</v>
+      </c>
+      <c r="F60" t="s">
         <v>166</v>
-      </c>
-      <c r="F60" t="s">
-        <v>167</v>
       </c>
       <c r="G60" t="s">
         <v>11</v>
@@ -2284,19 +2659,19 @@
         <v>120</v>
       </c>
       <c r="B61" t="s">
+        <v>167</v>
+      </c>
+      <c r="C61" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s">
+        <v>232</v>
+      </c>
+      <c r="F61" t="s">
         <v>168</v>
-      </c>
-      <c r="C61" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" t="s">
-        <v>15</v>
-      </c>
-      <c r="E61" t="s">
-        <v>166</v>
-      </c>
-      <c r="F61" t="s">
-        <v>169</v>
       </c>
       <c r="G61" t="s">
         <v>11</v>
@@ -2307,19 +2682,19 @@
         <v>120</v>
       </c>
       <c r="B62" t="s">
+        <v>169</v>
+      </c>
+      <c r="C62" t="s">
         <v>170</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" t="s">
         <v>171</v>
       </c>
-      <c r="D62" t="s">
-        <v>15</v>
-      </c>
-      <c r="E62" t="s">
-        <v>172</v>
-      </c>
       <c r="F62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G62" t="s">
         <v>11</v>
@@ -2330,19 +2705,19 @@
         <v>120</v>
       </c>
       <c r="B63" t="s">
+        <v>173</v>
+      </c>
+      <c r="C63" t="s">
         <v>174</v>
       </c>
-      <c r="C63" t="s">
-        <v>175</v>
-      </c>
       <c r="D63" t="s">
         <v>15</v>
       </c>
       <c r="E63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G63" t="s">
         <v>37</v>
@@ -2353,16 +2728,16 @@
         <v>120</v>
       </c>
       <c r="B64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D64" t="s">
         <v>8</v>
       </c>
       <c r="F64" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G64" t="s">
         <v>37</v>
@@ -2373,16 +2748,16 @@
         <v>120</v>
       </c>
       <c r="B65" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" t="s">
         <v>178</v>
       </c>
-      <c r="C65" t="s">
-        <v>179</v>
-      </c>
       <c r="D65" t="s">
         <v>8</v>
       </c>
       <c r="F65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G65" t="s">
         <v>37</v>
@@ -2393,16 +2768,16 @@
         <v>120</v>
       </c>
       <c r="B66" t="s">
+        <v>179</v>
+      </c>
+      <c r="C66" t="s">
         <v>180</v>
       </c>
-      <c r="C66" t="s">
-        <v>181</v>
-      </c>
       <c r="D66" t="s">
         <v>8</v>
       </c>
       <c r="F66" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G66" t="s">
         <v>37</v>
@@ -2413,16 +2788,16 @@
         <v>120</v>
       </c>
       <c r="B67" t="s">
+        <v>181</v>
+      </c>
+      <c r="C67" t="s">
         <v>182</v>
       </c>
-      <c r="C67" t="s">
-        <v>183</v>
-      </c>
       <c r="D67" t="s">
         <v>8</v>
       </c>
       <c r="F67" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G67" t="s">
         <v>37</v>
@@ -2433,16 +2808,16 @@
         <v>120</v>
       </c>
       <c r="B68" t="s">
+        <v>183</v>
+      </c>
+      <c r="C68" t="s">
         <v>184</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" t="s">
         <v>185</v>
-      </c>
-      <c r="D68" t="s">
-        <v>8</v>
-      </c>
-      <c r="F68" t="s">
-        <v>186</v>
       </c>
       <c r="G68" t="s">
         <v>37</v>
@@ -2453,16 +2828,16 @@
         <v>120</v>
       </c>
       <c r="B69" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" t="s">
         <v>193</v>
-      </c>
-      <c r="C69" t="s">
-        <v>194</v>
       </c>
       <c r="D69" t="s">
         <v>40</v>
       </c>
       <c r="F69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G69" t="s">
         <v>37</v>
@@ -2473,16 +2848,16 @@
         <v>120</v>
       </c>
       <c r="B70" t="s">
+        <v>195</v>
+      </c>
+      <c r="C70" t="s">
         <v>196</v>
-      </c>
-      <c r="C70" t="s">
-        <v>197</v>
       </c>
       <c r="D70" t="s">
         <v>40</v>
       </c>
       <c r="F70" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G70" t="s">
         <v>37</v>
@@ -2493,16 +2868,16 @@
         <v>120</v>
       </c>
       <c r="B71" t="s">
+        <v>198</v>
+      </c>
+      <c r="C71" t="s">
         <v>199</v>
-      </c>
-      <c r="C71" t="s">
-        <v>200</v>
       </c>
       <c r="D71" t="s">
         <v>40</v>
       </c>
       <c r="F71" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G71" t="s">
         <v>37</v>
@@ -2513,16 +2888,16 @@
         <v>120</v>
       </c>
       <c r="B72" t="s">
+        <v>201</v>
+      </c>
+      <c r="C72" t="s">
         <v>202</v>
-      </c>
-      <c r="C72" t="s">
-        <v>203</v>
       </c>
       <c r="D72" t="s">
         <v>40</v>
       </c>
       <c r="F72" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G72" t="s">
         <v>37</v>
@@ -2533,16 +2908,16 @@
         <v>120</v>
       </c>
       <c r="B73" t="s">
+        <v>204</v>
+      </c>
+      <c r="C73" t="s">
         <v>205</v>
-      </c>
-      <c r="C73" t="s">
-        <v>206</v>
       </c>
       <c r="D73" t="s">
         <v>40</v>
       </c>
       <c r="F73" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G73" t="s">
         <v>37</v>
@@ -2553,18 +2928,893 @@
         <v>120</v>
       </c>
       <c r="B74" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" t="s">
         <v>208</v>
-      </c>
-      <c r="C74" t="s">
-        <v>209</v>
       </c>
       <c r="D74" t="s">
         <v>40</v>
       </c>
       <c r="F74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G74" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>214</v>
+      </c>
+      <c r="B75" t="s">
+        <v>215</v>
+      </c>
+      <c r="C75" t="s">
+        <v>216</v>
+      </c>
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" t="s">
+        <v>217</v>
+      </c>
+      <c r="G75" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>214</v>
+      </c>
+      <c r="B76" t="s">
+        <v>218</v>
+      </c>
+      <c r="C76" t="s">
+        <v>219</v>
+      </c>
+      <c r="D76" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" t="s">
+        <v>220</v>
+      </c>
+      <c r="F76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G76" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>214</v>
+      </c>
+      <c r="B77" t="s">
+        <v>222</v>
+      </c>
+      <c r="C77" t="s">
+        <v>223</v>
+      </c>
+      <c r="D77" t="s">
+        <v>15</v>
+      </c>
+      <c r="E77" t="s">
+        <v>224</v>
+      </c>
+      <c r="F77" t="s">
+        <v>225</v>
+      </c>
+      <c r="G77" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>214</v>
+      </c>
+      <c r="B78" t="s">
+        <v>226</v>
+      </c>
+      <c r="C78" t="s">
+        <v>227</v>
+      </c>
+      <c r="D78" t="s">
+        <v>15</v>
+      </c>
+      <c r="E78" t="s">
+        <v>228</v>
+      </c>
+      <c r="F78" t="s">
+        <v>229</v>
+      </c>
+      <c r="G78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>214</v>
+      </c>
+      <c r="B79" t="s">
+        <v>231</v>
+      </c>
+      <c r="C79" t="s">
+        <v>230</v>
+      </c>
+      <c r="D79" t="s">
+        <v>15</v>
+      </c>
+      <c r="E79" t="s">
+        <v>234</v>
+      </c>
+      <c r="F79" t="s">
+        <v>233</v>
+      </c>
+      <c r="G79" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>214</v>
+      </c>
+      <c r="B80" t="s">
+        <v>235</v>
+      </c>
+      <c r="C80" t="s">
+        <v>240</v>
+      </c>
+      <c r="D80" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" t="s">
+        <v>246</v>
+      </c>
+      <c r="G80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>214</v>
+      </c>
+      <c r="B81" t="s">
+        <v>236</v>
+      </c>
+      <c r="C81" t="s">
+        <v>241</v>
+      </c>
+      <c r="D81" t="s">
+        <v>15</v>
+      </c>
+      <c r="E81" t="s">
+        <v>220</v>
+      </c>
+      <c r="F81" t="s">
+        <v>247</v>
+      </c>
+      <c r="G81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>214</v>
+      </c>
+      <c r="B82" t="s">
+        <v>237</v>
+      </c>
+      <c r="C82" t="s">
+        <v>242</v>
+      </c>
+      <c r="D82" t="s">
+        <v>15</v>
+      </c>
+      <c r="E82" t="s">
+        <v>224</v>
+      </c>
+      <c r="F82" t="s">
+        <v>248</v>
+      </c>
+      <c r="G82" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>214</v>
+      </c>
+      <c r="B83" t="s">
+        <v>238</v>
+      </c>
+      <c r="C83" t="s">
+        <v>243</v>
+      </c>
+      <c r="D83" t="s">
+        <v>15</v>
+      </c>
+      <c r="E83" t="s">
+        <v>228</v>
+      </c>
+      <c r="F83" t="s">
+        <v>249</v>
+      </c>
+      <c r="G83" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>214</v>
+      </c>
+      <c r="B84" t="s">
+        <v>239</v>
+      </c>
+      <c r="C84" t="s">
+        <v>244</v>
+      </c>
+      <c r="D84" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84" t="s">
+        <v>234</v>
+      </c>
+      <c r="F84" t="s">
+        <v>245</v>
+      </c>
+      <c r="G84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>214</v>
+      </c>
+      <c r="B85" t="s">
+        <v>250</v>
+      </c>
+      <c r="C85" t="s">
+        <v>255</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" t="s">
+        <v>256</v>
+      </c>
+      <c r="G85" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>214</v>
+      </c>
+      <c r="B86" t="s">
+        <v>251</v>
+      </c>
+      <c r="C86" t="s">
+        <v>257</v>
+      </c>
+      <c r="D86" t="s">
+        <v>15</v>
+      </c>
+      <c r="E86" t="s">
+        <v>220</v>
+      </c>
+      <c r="F86" t="s">
+        <v>258</v>
+      </c>
+      <c r="G86" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>214</v>
+      </c>
+      <c r="B87" t="s">
+        <v>252</v>
+      </c>
+      <c r="C87" t="s">
+        <v>259</v>
+      </c>
+      <c r="D87" t="s">
+        <v>15</v>
+      </c>
+      <c r="E87" t="s">
+        <v>224</v>
+      </c>
+      <c r="F87" t="s">
+        <v>260</v>
+      </c>
+      <c r="G87" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>214</v>
+      </c>
+      <c r="B88" t="s">
+        <v>253</v>
+      </c>
+      <c r="C88" t="s">
+        <v>261</v>
+      </c>
+      <c r="D88" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88" t="s">
+        <v>228</v>
+      </c>
+      <c r="F88" t="s">
+        <v>262</v>
+      </c>
+      <c r="G88" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>214</v>
+      </c>
+      <c r="B89" t="s">
+        <v>254</v>
+      </c>
+      <c r="C89" t="s">
+        <v>263</v>
+      </c>
+      <c r="D89" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" t="s">
+        <v>234</v>
+      </c>
+      <c r="F89" t="s">
+        <v>264</v>
+      </c>
+      <c r="G89" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>214</v>
+      </c>
+      <c r="B90" t="s">
+        <v>265</v>
+      </c>
+      <c r="C90" t="s">
+        <v>270</v>
+      </c>
+      <c r="D90" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" t="s">
+        <v>271</v>
+      </c>
+      <c r="G90" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>214</v>
+      </c>
+      <c r="B91" t="s">
+        <v>266</v>
+      </c>
+      <c r="C91" t="s">
+        <v>272</v>
+      </c>
+      <c r="D91" t="s">
+        <v>15</v>
+      </c>
+      <c r="E91" t="s">
+        <v>220</v>
+      </c>
+      <c r="F91" t="s">
+        <v>273</v>
+      </c>
+      <c r="G91" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>214</v>
+      </c>
+      <c r="B92" t="s">
+        <v>267</v>
+      </c>
+      <c r="C92" t="s">
+        <v>274</v>
+      </c>
+      <c r="D92" t="s">
+        <v>15</v>
+      </c>
+      <c r="E92" t="s">
+        <v>224</v>
+      </c>
+      <c r="F92" t="s">
+        <v>275</v>
+      </c>
+      <c r="G92" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>214</v>
+      </c>
+      <c r="B93" t="s">
+        <v>268</v>
+      </c>
+      <c r="C93" t="s">
+        <v>276</v>
+      </c>
+      <c r="D93" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" t="s">
+        <v>228</v>
+      </c>
+      <c r="F93" t="s">
+        <v>277</v>
+      </c>
+      <c r="G93" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>214</v>
+      </c>
+      <c r="B94" t="s">
+        <v>269</v>
+      </c>
+      <c r="C94" t="s">
+        <v>278</v>
+      </c>
+      <c r="D94" t="s">
+        <v>15</v>
+      </c>
+      <c r="E94" t="s">
+        <v>234</v>
+      </c>
+      <c r="F94" t="s">
+        <v>279</v>
+      </c>
+      <c r="G94" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>214</v>
+      </c>
+      <c r="B95" t="s">
+        <v>280</v>
+      </c>
+      <c r="C95" t="s">
+        <v>285</v>
+      </c>
+      <c r="D95" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" t="s">
+        <v>286</v>
+      </c>
+      <c r="G95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>214</v>
+      </c>
+      <c r="B96" t="s">
+        <v>281</v>
+      </c>
+      <c r="C96" t="s">
+        <v>287</v>
+      </c>
+      <c r="D96" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96" t="s">
+        <v>220</v>
+      </c>
+      <c r="F96" t="s">
+        <v>288</v>
+      </c>
+      <c r="G96" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>214</v>
+      </c>
+      <c r="B97" t="s">
+        <v>282</v>
+      </c>
+      <c r="C97" t="s">
+        <v>289</v>
+      </c>
+      <c r="D97" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97" t="s">
+        <v>224</v>
+      </c>
+      <c r="F97" t="s">
+        <v>290</v>
+      </c>
+      <c r="G97" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>214</v>
+      </c>
+      <c r="B98" t="s">
+        <v>283</v>
+      </c>
+      <c r="C98" t="s">
+        <v>291</v>
+      </c>
+      <c r="D98" t="s">
+        <v>15</v>
+      </c>
+      <c r="E98" t="s">
+        <v>228</v>
+      </c>
+      <c r="F98" t="s">
+        <v>292</v>
+      </c>
+      <c r="G98" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>214</v>
+      </c>
+      <c r="B99" t="s">
+        <v>284</v>
+      </c>
+      <c r="C99" t="s">
+        <v>293</v>
+      </c>
+      <c r="D99" t="s">
+        <v>15</v>
+      </c>
+      <c r="E99" t="s">
+        <v>234</v>
+      </c>
+      <c r="F99" t="s">
+        <v>294</v>
+      </c>
+      <c r="G99" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>214</v>
+      </c>
+      <c r="B100" t="s">
+        <v>295</v>
+      </c>
+      <c r="C100" t="s">
+        <v>300</v>
+      </c>
+      <c r="D100" t="s">
+        <v>8</v>
+      </c>
+      <c r="F100" t="s">
+        <v>301</v>
+      </c>
+      <c r="G100" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>214</v>
+      </c>
+      <c r="B101" t="s">
+        <v>296</v>
+      </c>
+      <c r="C101" t="s">
+        <v>302</v>
+      </c>
+      <c r="D101" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" t="s">
+        <v>220</v>
+      </c>
+      <c r="F101" t="s">
+        <v>303</v>
+      </c>
+      <c r="G101" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>214</v>
+      </c>
+      <c r="B102" t="s">
+        <v>297</v>
+      </c>
+      <c r="C102" t="s">
+        <v>304</v>
+      </c>
+      <c r="D102" t="s">
+        <v>15</v>
+      </c>
+      <c r="E102" t="s">
+        <v>224</v>
+      </c>
+      <c r="F102" t="s">
+        <v>305</v>
+      </c>
+      <c r="G102" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>214</v>
+      </c>
+      <c r="B103" t="s">
+        <v>298</v>
+      </c>
+      <c r="C103" t="s">
+        <v>306</v>
+      </c>
+      <c r="D103" t="s">
+        <v>15</v>
+      </c>
+      <c r="E103" t="s">
+        <v>228</v>
+      </c>
+      <c r="F103" t="s">
+        <v>307</v>
+      </c>
+      <c r="G103" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>214</v>
+      </c>
+      <c r="B104" t="s">
+        <v>299</v>
+      </c>
+      <c r="C104" t="s">
+        <v>308</v>
+      </c>
+      <c r="D104" t="s">
+        <v>15</v>
+      </c>
+      <c r="E104" t="s">
+        <v>234</v>
+      </c>
+      <c r="F104" t="s">
+        <v>309</v>
+      </c>
+      <c r="G104" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>214</v>
+      </c>
+      <c r="B105" t="s">
+        <v>310</v>
+      </c>
+      <c r="C105" t="s">
+        <v>311</v>
+      </c>
+      <c r="D105" t="s">
+        <v>105</v>
+      </c>
+      <c r="F105" t="s">
+        <v>312</v>
+      </c>
+      <c r="G105" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>214</v>
+      </c>
+      <c r="B106" t="s">
+        <v>313</v>
+      </c>
+      <c r="C106" t="s">
+        <v>314</v>
+      </c>
+      <c r="D106" t="s">
+        <v>105</v>
+      </c>
+      <c r="F106" t="s">
+        <v>329</v>
+      </c>
+      <c r="G106" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>214</v>
+      </c>
+      <c r="B107" t="s">
+        <v>315</v>
+      </c>
+      <c r="C107" t="s">
+        <v>316</v>
+      </c>
+      <c r="D107" t="s">
+        <v>105</v>
+      </c>
+      <c r="F107" t="s">
+        <v>328</v>
+      </c>
+      <c r="G107" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>317</v>
+      </c>
+      <c r="C108" t="s">
+        <v>318</v>
+      </c>
+      <c r="D108" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" t="s">
+        <v>220</v>
+      </c>
+      <c r="F108" t="s">
+        <v>319</v>
+      </c>
+      <c r="G108" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>214</v>
+      </c>
+      <c r="B109" t="s">
+        <v>320</v>
+      </c>
+      <c r="C109" t="s">
+        <v>321</v>
+      </c>
+      <c r="D109" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" t="s">
+        <v>326</v>
+      </c>
+      <c r="G109" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>214</v>
+      </c>
+      <c r="B110" t="s">
+        <v>322</v>
+      </c>
+      <c r="C110" t="s">
+        <v>323</v>
+      </c>
+      <c r="D110" t="s">
+        <v>15</v>
+      </c>
+      <c r="F110" t="s">
+        <v>327</v>
+      </c>
+      <c r="G110" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>214</v>
+      </c>
+      <c r="B111" t="s">
+        <v>324</v>
+      </c>
+      <c r="C111" t="s">
+        <v>325</v>
+      </c>
+      <c r="D111" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" t="s">
+        <v>339</v>
+      </c>
+      <c r="G111" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>214</v>
+      </c>
+      <c r="B112" t="s">
+        <v>330</v>
+      </c>
+      <c r="C112" t="s">
+        <v>331</v>
+      </c>
+      <c r="D112" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" t="s">
+        <v>332</v>
+      </c>
+      <c r="G112" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>214</v>
+      </c>
+      <c r="B113" t="s">
+        <v>333</v>
+      </c>
+      <c r="C113" t="s">
+        <v>334</v>
+      </c>
+      <c r="D113" t="s">
+        <v>40</v>
+      </c>
+      <c r="F113" t="s">
+        <v>335</v>
+      </c>
+      <c r="G113" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>214</v>
+      </c>
+      <c r="B114" t="s">
+        <v>336</v>
+      </c>
+      <c r="C114" t="s">
+        <v>337</v>
+      </c>
+      <c r="D114" t="s">
+        <v>8</v>
+      </c>
+      <c r="F114" t="s">
+        <v>338</v>
+      </c>
+      <c r="G114" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add parameters of measure add_ideal_loads to argument table.
</commit_message>
<xml_diff>
--- a/docs/Measure_Arguments.xlsx
+++ b/docs/Measure_Arguments.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="341">
   <si>
     <t>Measure</t>
   </si>
@@ -1047,6 +1047,9 @@
   </si>
   <si>
     <t>Solar heat gain coefficient of the windows constructions.</t>
+  </si>
+  <si>
+    <t>add_ideal_loads</t>
   </si>
 </sst>
 </file>
@@ -1365,10 +1368,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3778,7 +3781,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>214</v>
       </c>
@@ -3798,7 +3801,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>214</v>
       </c>
@@ -3815,6 +3818,287 @@
         <v>338</v>
       </c>
       <c r="G114" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>340</v>
+      </c>
+      <c r="B115" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s">
+        <v>95</v>
+      </c>
+      <c r="D115" t="s">
+        <v>8</v>
+      </c>
+      <c r="F115" t="s">
+        <v>9</v>
+      </c>
+      <c r="G115" t="s">
+        <v>11</v>
+      </c>
+      <c r="H115" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>340</v>
+      </c>
+      <c r="B116" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" t="s">
+        <v>15</v>
+      </c>
+      <c r="F116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G116" t="s">
+        <v>11</v>
+      </c>
+      <c r="H116" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>340</v>
+      </c>
+      <c r="B117" t="s">
+        <v>18</v>
+      </c>
+      <c r="C117" t="s">
+        <v>19</v>
+      </c>
+      <c r="D117" t="s">
+        <v>15</v>
+      </c>
+      <c r="F117" t="s">
+        <v>20</v>
+      </c>
+      <c r="G117" t="s">
+        <v>11</v>
+      </c>
+      <c r="H117" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>340</v>
+      </c>
+      <c r="B118" t="s">
+        <v>23</v>
+      </c>
+      <c r="C118" t="s">
+        <v>24</v>
+      </c>
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" t="s">
+        <v>25</v>
+      </c>
+      <c r="F118" t="s">
+        <v>26</v>
+      </c>
+      <c r="G118" t="s">
+        <v>11</v>
+      </c>
+      <c r="H118" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>340</v>
+      </c>
+      <c r="B119" t="s">
+        <v>28</v>
+      </c>
+      <c r="C119" t="s">
+        <v>29</v>
+      </c>
+      <c r="D119" t="s">
+        <v>15</v>
+      </c>
+      <c r="F119" t="s">
+        <v>30</v>
+      </c>
+      <c r="G119" t="s">
+        <v>11</v>
+      </c>
+      <c r="H119" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>340</v>
+      </c>
+      <c r="B120" t="s">
+        <v>31</v>
+      </c>
+      <c r="C120" t="s">
+        <v>32</v>
+      </c>
+      <c r="D120" t="s">
+        <v>15</v>
+      </c>
+      <c r="F120" t="s">
+        <v>33</v>
+      </c>
+      <c r="G120" t="s">
+        <v>11</v>
+      </c>
+      <c r="H120" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>340</v>
+      </c>
+      <c r="B121" t="s">
+        <v>34</v>
+      </c>
+      <c r="C121" t="s">
+        <v>35</v>
+      </c>
+      <c r="D121" t="s">
+        <v>8</v>
+      </c>
+      <c r="F121" t="s">
+        <v>36</v>
+      </c>
+      <c r="G121" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>340</v>
+      </c>
+      <c r="B122" t="s">
+        <v>38</v>
+      </c>
+      <c r="C122" t="s">
+        <v>39</v>
+      </c>
+      <c r="D122" t="s">
+        <v>40</v>
+      </c>
+      <c r="F122" t="s">
+        <v>41</v>
+      </c>
+      <c r="G122" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>340</v>
+      </c>
+      <c r="B123" t="s">
+        <v>42</v>
+      </c>
+      <c r="C123" t="s">
+        <v>43</v>
+      </c>
+      <c r="D123" t="s">
+        <v>8</v>
+      </c>
+      <c r="F123" t="s">
+        <v>44</v>
+      </c>
+      <c r="G123" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>340</v>
+      </c>
+      <c r="B124" t="s">
+        <v>45</v>
+      </c>
+      <c r="C124" t="s">
+        <v>46</v>
+      </c>
+      <c r="D124" t="s">
+        <v>8</v>
+      </c>
+      <c r="F124" t="s">
+        <v>47</v>
+      </c>
+      <c r="G124" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>340</v>
+      </c>
+      <c r="B125" t="s">
+        <v>48</v>
+      </c>
+      <c r="C125" t="s">
+        <v>49</v>
+      </c>
+      <c r="D125" t="s">
+        <v>8</v>
+      </c>
+      <c r="F125" t="s">
+        <v>50</v>
+      </c>
+      <c r="G125" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>340</v>
+      </c>
+      <c r="B126" t="s">
+        <v>51</v>
+      </c>
+      <c r="C126" t="s">
+        <v>52</v>
+      </c>
+      <c r="D126" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" t="s">
+        <v>53</v>
+      </c>
+      <c r="G126" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>340</v>
+      </c>
+      <c r="B127" t="s">
+        <v>66</v>
+      </c>
+      <c r="C127" t="s">
+        <v>67</v>
+      </c>
+      <c r="D127" t="s">
+        <v>8</v>
+      </c>
+      <c r="F127" t="s">
+        <v>68</v>
+      </c>
+      <c r="G127" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename measure argument hvac_schedule to hvac_sched_selection for improved consistency across arguments.
</commit_message>
<xml_diff>
--- a/docs/Measure_Arguments.xlsx
+++ b/docs/Measure_Arguments.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="473">
   <si>
     <t>Measure</t>
   </si>
@@ -1440,6 +1440,12 @@
   </si>
   <si>
     <t>Flag whether the selected cooling temperature is a custom schedule</t>
+  </si>
+  <si>
+    <t>hvac_sched_selection</t>
+  </si>
+  <si>
+    <t>Selection value of the HVAC schedule</t>
   </si>
 </sst>
 </file>
@@ -1762,7 +1768,7 @@
   <dimension ref="A1:I188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,7 +2128,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>471</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
@@ -2131,7 +2137,7 @@
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>317</v>
+        <v>472</v>
       </c>
       <c r="G14" t="s">
         <v>32</v>

</xml_diff>